<commit_message>
corrections scripts for data model
</commit_message>
<xml_diff>
--- a/data/Spreadsheet_Data/Location.xlsx
+++ b/data/Spreadsheet_Data/Location.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noemivillars-amberg/Documents/daschland-scripts/data/Spreadsheet_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91662DFA-6778-4A49-9199-FFF000894E77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E0F988B-1E8E-084B-AB4A-0E830F2F8474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="42080" yWindow="500" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="29">
   <si>
     <t>L_001</t>
   </si>
@@ -91,40 +91,22 @@
     <t>ID</t>
   </si>
   <si>
-    <t>Geoname</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
-    <t>Wonderland Location List</t>
-  </si>
-  <si>
-    <t>Location 1</t>
-  </si>
-  <si>
-    <t>Location 2</t>
-  </si>
-  <si>
-    <t>Location 3</t>
-  </si>
-  <si>
-    <t>Location 4</t>
-  </si>
-  <si>
-    <t>Location 5</t>
-  </si>
-  <si>
-    <t>Location 6</t>
-  </si>
-  <si>
-    <t>Location 7</t>
-  </si>
-  <si>
-    <t>Location 8</t>
-  </si>
-  <si>
-    <t>Location 9</t>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Geoname ID</t>
+  </si>
+  <si>
+    <t>Location Type List</t>
+  </si>
+  <si>
+    <t>Real World</t>
+  </si>
+  <si>
+    <t>Wonderland</t>
   </si>
 </sst>
 </file>
@@ -431,254 +413,277 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.6640625" style="2"/>
-    <col min="2" max="2" width="25.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="27.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="28.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="12.6640625" style="2"/>
+    <col min="2" max="2" width="27.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="28.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5" style="2" customWidth="1"/>
+    <col min="5" max="5" width="34" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="12.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="C2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="C3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="C4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="C5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="C6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="C7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="C8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="C9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="C10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="1">
-        <v>2640729</v>
+      <c r="B11" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="1">
+        <v>2640729</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="1">
-        <v>6269131</v>
+      <c r="B12" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="1">
+        <v>6269131</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="5"/>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="4"/>
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="6"/>
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="1"/>
+      <c r="E26" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>